<commit_message>
Added API and Load test cases
</commit_message>
<xml_diff>
--- a/API Tests and Load Test/API_Test Cases_V1.0.xlsx
+++ b/API Tests and Load Test/API_Test Cases_V1.0.xlsx
@@ -773,7 +773,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>447035</xdr:colOff>
+      <xdr:colOff>567685</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>18228</xdr:rowOff>
     </xdr:to>
@@ -1060,7 +1060,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1772,13 +1772,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+    <col min="1" max="1" width="24.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="32.44140625" customWidth="1"/>
     <col min="4" max="4" width="29.21875" customWidth="1"/>

</xml_diff>